<commit_message>
Add Scythe in UI
</commit_message>
<xml_diff>
--- a/assests_extra/recepies.XLSX
+++ b/assests_extra/recepies.XLSX
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\EmpireBuilder\assests_extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C95A016-73F3-46A0-A165-8259D900C9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78390F83-13EC-42F7-8181-F662136F3A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="1" r:id="rId1"/>
-    <sheet name="Buildings" sheetId="2" r:id="rId2"/>
+    <sheet name="Tools" sheetId="4" r:id="rId2"/>
+    <sheet name="Buildings" sheetId="2" r:id="rId3"/>
+    <sheet name="Bonus" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
   <si>
     <t>Berry Bush</t>
   </si>
@@ -137,6 +139,72 @@
   </si>
   <si>
     <t>Axe</t>
+  </si>
+  <si>
+    <t>Resource Name</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Tool Image</t>
+  </si>
+  <si>
+    <t>Bonus value</t>
+  </si>
+  <si>
+    <t>Bonus Time</t>
+  </si>
+  <si>
+    <t>scythe</t>
+  </si>
+  <si>
+    <t>Fishing pond</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Building image</t>
+  </si>
+  <si>
+    <t>Fishing Hut lvl 0</t>
+  </si>
+  <si>
+    <t>Herbalist Hut lvl 0</t>
+  </si>
+  <si>
+    <t>Bonus Key</t>
+  </si>
+  <si>
+    <t>Clayworker Hut lvl 0</t>
+  </si>
+  <si>
+    <t>tool index</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Sticks</t>
+  </si>
+  <si>
+    <t>PickAxe lvl 0</t>
+  </si>
+  <si>
+    <t>Spear lvl 0</t>
+  </si>
+  <si>
+    <t>Axe lvl 0</t>
+  </si>
+  <si>
+    <t>Scythe lvl 0</t>
   </si>
 </sst>
 </file>
@@ -168,7 +236,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -262,11 +330,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -322,6 +412,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1443,13 +1569,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>361950</xdr:rowOff>
@@ -1493,13 +1619,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
@@ -1643,13 +1769,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>342900</xdr:rowOff>
@@ -1683,6 +1809,986 @@
         <a:xfrm>
           <a:off x="6467475" y="4819650"/>
           <a:ext cx="390525" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C9591C5-FE60-45E0-B98C-2472E839C5E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="190500"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{365895C3-A6E1-4DE4-BAC5-03CE7987806B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3619500" y="104775"/>
+          <a:ext cx="400050" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>353020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC123F9A-9172-41FC-AF1B-098E624B5E2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3590925" y="561975"/>
+          <a:ext cx="400050" cy="362545"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3419D993-C6E8-4368-A944-ED68BB15CA99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1038225" y="962025"/>
+          <a:ext cx="361950" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="400050"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD4C1AF9-B2C8-426C-91F8-CCBE19B28473}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3705225" y="876300"/>
+          <a:ext cx="400050" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="362545"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50DFB55B-6B87-4FD6-9624-28234881CC82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3695700" y="561975"/>
+          <a:ext cx="400050" cy="362545"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEBC0E59-F615-40B0-A1A3-B178F7877F81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1019175" y="1685925"/>
+          <a:ext cx="381000" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="400050"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06891757-BA46-4F7F-BED3-FC8392F4F857}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3705225" y="876300"/>
+          <a:ext cx="400050" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="362545"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{785F5390-D20E-4D90-A304-EAA5E94CC5B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3695700" y="1323975"/>
+          <a:ext cx="400050" cy="362545"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B32E05E-7709-4040-A494-582A83071359}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1019175" y="2524125"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="400050"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A1322CA-1ADA-48FE-A483-9F66D26950FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3705225" y="1638300"/>
+          <a:ext cx="400050" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="362545"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DE599BA-DFAF-4DC9-9FCC-94A9F24A9B09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3695700" y="2095500"/>
+          <a:ext cx="400050" cy="362545"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>219074</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>304799</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14665446-11EC-49A4-A29B-B894DADF95E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="219074"/>
+          <a:ext cx="514350" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A82A503A-2063-44A0-86A2-FEFA6EEC60FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3600450" y="409575"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFD1ECDE-A0A6-4BCC-9B6E-C0D823A31272}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1352550" y="600075"/>
+          <a:ext cx="476250" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29BFF728-CDD0-4F96-BEA5-5A5AF15F6D39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5505450" y="609600"/>
+          <a:ext cx="523875" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4E7EA79-DBB7-4518-9515-2DF61E8276C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1438275" y="1123950"/>
+          <a:ext cx="371475" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1042A42A-7C9A-4359-926C-DC74C423113D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5438775" y="962025"/>
+          <a:ext cx="533400" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BD529F7-7980-4EDA-86D6-FC251C55E66D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="1428750"/>
+          <a:ext cx="457200" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8DDB998-318F-4A64-98EB-786D78EBDBB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5686425" y="1371600"/>
+          <a:ext cx="504825" cy="504825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1957,10 +3063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1971,12 +3077,14 @@
     <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
-    <col min="7" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="15.7109375" style="21" customWidth="1"/>
+    <col min="10" max="12" width="9.140625" style="1"/>
+    <col min="13" max="16" width="17.85546875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1996,22 +3104,26 @@
         <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
@@ -2029,21 +3141,25 @@
         <v>9</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="K2" s="4"/>
       <c r="L2" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
     </row>
-    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>12</v>
       </c>
@@ -2061,21 +3177,25 @@
         <v>13</v>
       </c>
       <c r="G3" s="7"/>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7">
-        <v>1</v>
-      </c>
-      <c r="K3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="K3" s="7"/>
       <c r="L3" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
     </row>
-    <row r="4" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>14</v>
       </c>
@@ -2093,21 +3213,25 @@
         <v>15</v>
       </c>
       <c r="G4" s="7"/>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="7">
+        <v>2</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7">
-        <v>2</v>
-      </c>
-      <c r="K4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="K4" s="7"/>
       <c r="L4" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
     </row>
-    <row r="5" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -2119,19 +3243,23 @@
         <v>17</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9">
+      <c r="H5" s="9">
         <v>4</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="I5" s="21" t="s">
         <v>10</v>
       </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
       <c r="L5" s="11" t="s">
         <v>10</v>
       </c>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
     </row>
-    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -2148,19 +3276,23 @@
         <v>18</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="21">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="1">
-        <v>6</v>
       </c>
       <c r="L6" s="12">
         <v>1</v>
       </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
     </row>
-    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -2172,19 +3304,23 @@
         <v>19</v>
       </c>
       <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13" t="s">
+      <c r="H7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="13">
+      <c r="I7" s="13">
         <v>5</v>
       </c>
-      <c r="L7" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="14">
+        <v>5</v>
+      </c>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
     </row>
-    <row r="8" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>21</v>
       </c>
@@ -2202,21 +3338,25 @@
         <v>22</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="7">
+        <v>3</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7">
-        <v>3</v>
-      </c>
-      <c r="K8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="K8" s="7"/>
       <c r="L8" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
     </row>
-    <row r="9" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>23</v>
       </c>
@@ -2237,18 +3377,22 @@
       <c r="H9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="J9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="7"/>
+      <c r="L9" s="8">
         <v>1</v>
       </c>
-      <c r="L9" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
     </row>
-    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>25</v>
       </c>
@@ -2269,18 +3413,22 @@
       <c r="H10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="J10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="7"/>
+      <c r="L10" s="8">
         <v>4</v>
       </c>
-      <c r="L10" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
     </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>27</v>
       </c>
@@ -2301,18 +3449,22 @@
       <c r="H11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="J11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="7"/>
+      <c r="L11" s="8">
         <v>0</v>
       </c>
-      <c r="L11" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
     </row>
-    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>29</v>
       </c>
@@ -2333,18 +3485,22 @@
       <c r="H12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="J12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="7"/>
+      <c r="L12" s="8">
         <v>3</v>
       </c>
-      <c r="L12" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
     </row>
-    <row r="13" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>31</v>
       </c>
@@ -2363,20 +3519,24 @@
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0</v>
+      </c>
+      <c r="J13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="7">
+      <c r="K13" s="7"/>
+      <c r="L13" s="8">
         <v>2</v>
       </c>
-      <c r="L13" s="8">
-        <v>0</v>
-      </c>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
     </row>
-    <row r="14" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>34</v>
       </c>
@@ -2395,18 +3555,22 @@
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="13">
+        <v>2</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="7">
+      <c r="K14" s="7"/>
+      <c r="L14" s="8">
         <v>7</v>
       </c>
-      <c r="L14" s="8">
-        <v>2</v>
-      </c>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2416,13 +3580,347 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD27627A-3A20-455E-B4FE-556EC041BC52}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16"/>
+      <c r="B1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9">
+        <v>2</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71D75D97-CC6F-43EE-A366-5B2B42E1B1E4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7293435B-1AF2-4E46-92A9-37C60DF01C2E}">
+  <dimension ref="A1:S5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="7">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7">
+        <v>50</v>
+      </c>
+      <c r="J2" s="14">
+        <v>3</v>
+      </c>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8">
+        <v>0</v>
+      </c>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8">
+        <v>1</v>
+      </c>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+    </row>
+    <row r="5" spans="1:19" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8">
+        <v>2</v>
+      </c>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>